<commit_message>
Filled in missing categories for 2 PIs
</commit_message>
<xml_diff>
--- a/EDITED_Primary_Category_for_each_PI.xlsx
+++ b/EDITED_Primary_Category_for_each_PI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keeganflanagan/Desktop/Brain_Circuits_Position/Diagram of DMCBH Connections/Chrod_diagram_R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolecheung/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29608AEA-A2A3-9942-B4DF-E360A1958FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61FA8938-6132-194A-BD60-6D0EFED69082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="500" windowWidth="23160" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="347">
   <si>
     <t xml:space="preserve">Last Name </t>
   </si>
@@ -723,9 +732,6 @@
     <t xml:space="preserve">Jane Roskams </t>
   </si>
   <si>
-    <t>Schütz</t>
-  </si>
-  <si>
     <t>Christian</t>
   </si>
   <si>
@@ -1060,6 +1066,15 @@
   </si>
   <si>
     <t>Joel Oger</t>
+  </si>
+  <si>
+    <t>Schuetz</t>
+  </si>
+  <si>
+    <t>Judy Illes</t>
+  </si>
+  <si>
+    <t>Tao Huan</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1727,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1755,7 +1770,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E1" s="42" t="s">
         <v>3</v>
@@ -2848,7 +2863,9 @@
         <v>106</v>
       </c>
       <c r="C35"/>
-      <c r="D35"/>
+      <c r="D35" s="59" t="s">
+        <v>346</v>
+      </c>
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35"/>
@@ -2881,7 +2898,9 @@
       <c r="D36"/>
       <c r="E36"/>
       <c r="F36"/>
-      <c r="G36"/>
+      <c r="G36" s="55" t="s">
+        <v>345</v>
+      </c>
       <c r="H36" s="67"/>
       <c r="I36" s="68"/>
       <c r="J36" s="67"/>
@@ -3775,7 +3794,7 @@
       <c r="D64"/>
       <c r="E64"/>
       <c r="F64" s="55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G64"/>
       <c r="H64" s="12"/>
@@ -4246,13 +4265,13 @@
     </row>
     <row r="79" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="B79" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="C79" s="61" t="s">
         <v>233</v>
-      </c>
-      <c r="C79" s="61" t="s">
-        <v>234</v>
       </c>
       <c r="D79"/>
       <c r="E79"/>
@@ -4278,13 +4297,13 @@
     </row>
     <row r="80" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="B80" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="B80" s="23" t="s">
+      <c r="C80" s="59" t="s">
         <v>236</v>
-      </c>
-      <c r="C80" s="59" t="s">
-        <v>237</v>
       </c>
       <c r="D80"/>
       <c r="E80"/>
@@ -4310,17 +4329,17 @@
     </row>
     <row r="81" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>239</v>
       </c>
       <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
       <c r="F81"/>
       <c r="G81" s="55" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H81" s="11"/>
       <c r="I81" s="11"/>
@@ -4342,7 +4361,7 @@
     </row>
     <row r="82" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>28</v>
@@ -4350,7 +4369,7 @@
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82" s="55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F82"/>
       <c r="G82"/>
@@ -4374,14 +4393,14 @@
     </row>
     <row r="83" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B83" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="C83"/>
       <c r="D83" s="55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E83"/>
       <c r="F83"/>
@@ -4406,15 +4425,15 @@
     </row>
     <row r="84" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B84" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>247</v>
       </c>
       <c r="C84"/>
       <c r="D84"/>
       <c r="E84" s="55" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F84"/>
       <c r="G84"/>
@@ -4438,16 +4457,16 @@
     </row>
     <row r="85" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>249</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="C85"/>
       <c r="D85"/>
       <c r="E85"/>
       <c r="F85" s="55" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G85"/>
       <c r="H85" s="11"/>
@@ -4470,16 +4489,16 @@
     </row>
     <row r="86" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" s="23" t="s">
         <v>252</v>
-      </c>
-      <c r="B86" s="23" t="s">
-        <v>253</v>
       </c>
       <c r="C86"/>
       <c r="D86"/>
       <c r="E86"/>
       <c r="F86" s="59" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G86"/>
       <c r="H86" s="12"/>
@@ -4502,16 +4521,16 @@
     </row>
     <row r="87" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="B87" s="23" t="s">
         <v>255</v>
-      </c>
-      <c r="B87" s="23" t="s">
-        <v>256</v>
       </c>
       <c r="C87"/>
       <c r="D87"/>
       <c r="E87"/>
       <c r="F87" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G87"/>
       <c r="H87" s="12"/>
@@ -4534,13 +4553,13 @@
     </row>
     <row r="88" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B88" s="23" t="s">
         <v>176</v>
       </c>
       <c r="C88" s="59" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D88"/>
       <c r="E88"/>
@@ -4566,13 +4585,13 @@
     </row>
     <row r="89" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="B89" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="B89" s="23" t="s">
+      <c r="C89" s="59" t="s">
         <v>261</v>
-      </c>
-      <c r="C89" s="59" t="s">
-        <v>262</v>
       </c>
       <c r="D89"/>
       <c r="E89"/>
@@ -4598,16 +4617,16 @@
     </row>
     <row r="90" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B90" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>264</v>
       </c>
       <c r="C90"/>
       <c r="D90"/>
       <c r="E90"/>
       <c r="F90" s="55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G90"/>
       <c r="H90" s="25"/>
@@ -4630,17 +4649,17 @@
     </row>
     <row r="91" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B91" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>267</v>
       </c>
       <c r="C91"/>
       <c r="D91"/>
       <c r="E91"/>
       <c r="F91"/>
       <c r="G91" s="55" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H91" s="13"/>
       <c r="I91" s="13"/>
@@ -4662,13 +4681,13 @@
     </row>
     <row r="92" spans="1:24" s="65" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="B92" s="66" t="s">
         <v>269</v>
       </c>
-      <c r="B92" s="66" t="s">
+      <c r="C92" s="55" t="s">
         <v>270</v>
-      </c>
-      <c r="C92" s="55" t="s">
-        <v>271</v>
       </c>
       <c r="D92"/>
       <c r="E92"/>
@@ -4694,16 +4713,16 @@
     </row>
     <row r="93" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B93" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="C93"/>
       <c r="D93"/>
       <c r="E93"/>
       <c r="F93" s="55" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G93"/>
       <c r="H93" s="11"/>
@@ -4726,16 +4745,16 @@
     </row>
     <row r="94" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="C94"/>
       <c r="D94"/>
       <c r="E94"/>
       <c r="F94" s="55" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G94"/>
       <c r="H94" s="11"/>
@@ -4758,13 +4777,13 @@
     </row>
     <row r="95" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="B95" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="B95" s="23" t="s">
+      <c r="C95" s="59" t="s">
         <v>279</v>
-      </c>
-      <c r="C95" s="59" t="s">
-        <v>280</v>
       </c>
       <c r="D95"/>
       <c r="E95"/>
@@ -4790,7 +4809,7 @@
     </row>
     <row r="96" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>202</v>
@@ -4800,7 +4819,7 @@
       <c r="E96"/>
       <c r="F96"/>
       <c r="G96" s="55" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H96" s="13"/>
       <c r="I96" s="13"/>
@@ -4822,13 +4841,13 @@
     </row>
     <row r="97" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B97" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="C97" s="55" t="s">
         <v>284</v>
-      </c>
-      <c r="C97" s="55" t="s">
-        <v>285</v>
       </c>
       <c r="D97"/>
       <c r="E97"/>
@@ -4854,13 +4873,13 @@
     </row>
     <row r="98" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="B98" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="B98" s="23" t="s">
+      <c r="C98" s="59" t="s">
         <v>287</v>
-      </c>
-      <c r="C98" s="59" t="s">
-        <v>288</v>
       </c>
       <c r="D98"/>
       <c r="E98"/>
@@ -4886,16 +4905,16 @@
     </row>
     <row r="99" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B99" s="6" t="s">
         <v>289</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="C99"/>
       <c r="D99"/>
       <c r="E99"/>
       <c r="F99" s="55" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G99"/>
       <c r="H99" s="11"/>
@@ -4918,13 +4937,13 @@
     </row>
     <row r="100" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B100" s="6" t="s">
+      <c r="C100" s="55" t="s">
         <v>293</v>
-      </c>
-      <c r="C100" s="55" t="s">
-        <v>294</v>
       </c>
       <c r="D100"/>
       <c r="E100"/>
@@ -4950,17 +4969,17 @@
     </row>
     <row r="101" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B101" s="6" t="s">
         <v>295</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>296</v>
       </c>
       <c r="C101"/>
       <c r="D101"/>
       <c r="E101"/>
       <c r="F101"/>
       <c r="G101" s="55" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H101" s="13"/>
       <c r="I101" s="13"/>
@@ -4982,17 +5001,17 @@
     </row>
     <row r="102" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B102" s="6" t="s">
         <v>298</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>299</v>
       </c>
       <c r="C102"/>
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
       <c r="G102" s="55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H102" s="11"/>
       <c r="I102" s="11"/>
@@ -5014,15 +5033,15 @@
     </row>
     <row r="103" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="B103" s="23" t="s">
         <v>301</v>
-      </c>
-      <c r="B103" s="23" t="s">
-        <v>302</v>
       </c>
       <c r="C103"/>
       <c r="D103"/>
       <c r="E103" s="59" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F103"/>
       <c r="G103"/>
@@ -5046,17 +5065,17 @@
     </row>
     <row r="104" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>305</v>
       </c>
       <c r="C104"/>
       <c r="D104"/>
       <c r="E104"/>
       <c r="F104"/>
       <c r="G104" s="55" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H104" s="11"/>
       <c r="I104" s="11"/>
@@ -5078,14 +5097,14 @@
     </row>
     <row r="105" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B105" s="6" t="s">
         <v>307</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>308</v>
       </c>
       <c r="C105"/>
       <c r="D105" s="55" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E105"/>
       <c r="F105"/>
@@ -5110,13 +5129,13 @@
     </row>
     <row r="106" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>216</v>
       </c>
       <c r="C106" s="55" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D106"/>
       <c r="E106"/>
@@ -5142,13 +5161,13 @@
     </row>
     <row r="107" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C107" s="55" t="s">
         <v>312</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="C107" s="55" t="s">
-        <v>313</v>
       </c>
       <c r="D107"/>
       <c r="E107"/>
@@ -5174,13 +5193,13 @@
     </row>
     <row r="108" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="23" t="s">
+        <v>313</v>
+      </c>
+      <c r="B108" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="B108" s="23" t="s">
+      <c r="C108" s="59" t="s">
         <v>315</v>
-      </c>
-      <c r="C108" s="59" t="s">
-        <v>316</v>
       </c>
       <c r="D108"/>
       <c r="E108"/>
@@ -5310,7 +5329,7 @@
     </row>
     <row r="113" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113"/>
@@ -5338,10 +5357,10 @@
     </row>
     <row r="114" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="B114" s="24" t="s">
         <v>318</v>
-      </c>
-      <c r="B114" s="24" t="s">
-        <v>319</v>
       </c>
       <c r="C114"/>
       <c r="D114"/>
@@ -5368,7 +5387,7 @@
     </row>
     <row r="115" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B115" s="23" t="s">
         <v>51</v>
@@ -5398,10 +5417,10 @@
     </row>
     <row r="116" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B116" s="6" t="s">
         <v>321</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>322</v>
       </c>
       <c r="C116"/>
       <c r="D116"/>
@@ -5428,10 +5447,10 @@
     </row>
     <row r="117" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B117" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>324</v>
       </c>
       <c r="C117"/>
       <c r="D117"/>
@@ -5458,10 +5477,10 @@
     </row>
     <row r="118" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="23" t="s">
+        <v>324</v>
+      </c>
+      <c r="B118" s="23" t="s">
         <v>325</v>
-      </c>
-      <c r="B118" s="23" t="s">
-        <v>326</v>
       </c>
       <c r="C118"/>
       <c r="D118"/>
@@ -5488,10 +5507,10 @@
     </row>
     <row r="119" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="B119" s="23" t="s">
         <v>327</v>
-      </c>
-      <c r="B119" s="23" t="s">
-        <v>328</v>
       </c>
       <c r="C119"/>
       <c r="D119"/>
@@ -5518,7 +5537,7 @@
     </row>
     <row r="120" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B120" s="23" t="s">
         <v>143</v>
@@ -5548,10 +5567,10 @@
     </row>
     <row r="121" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C121"/>
       <c r="D121"/>
@@ -5578,7 +5597,7 @@
     </row>
     <row r="122" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B122" s="23" t="s">
         <v>167</v>
@@ -5608,10 +5627,10 @@
     </row>
     <row r="123" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B123" s="6" t="s">
         <v>332</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>333</v>
       </c>
       <c r="C123"/>
       <c r="D123"/>
@@ -5638,10 +5657,10 @@
     </row>
     <row r="124" spans="1:24" s="34" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="B124" s="26" t="s">
         <v>334</v>
-      </c>
-      <c r="B124" s="26" t="s">
-        <v>335</v>
       </c>
       <c r="C124"/>
       <c r="D124"/>
@@ -5668,10 +5687,10 @@
     </row>
     <row r="125" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>336</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="C125"/>
       <c r="D125"/>
@@ -5698,10 +5717,10 @@
     </row>
     <row r="126" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B126" s="6" t="s">
         <v>338</v>
-      </c>
-      <c r="B126" s="6" t="s">
-        <v>339</v>
       </c>
       <c r="C126"/>
       <c r="D126"/>
@@ -5728,7 +5747,7 @@
     </row>
     <row r="127" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B127" s="39" t="s">
         <v>143</v>
@@ -5758,10 +5777,10 @@
     </row>
     <row r="128" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B128" s="6" t="s">
         <v>341</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>342</v>
       </c>
       <c r="C128"/>
       <c r="D128"/>
@@ -6131,6 +6150,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="a04c2f80-1bef-4486-925b-388b55f507c4">
@@ -6144,7 +6172,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003F67D3AF7D0E554F93D1DBE4789CF6A0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac5e5ad5c27f1eac4c90f38925cb47b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f799c52-a1b3-4ee5-ac1d-d25d561b6180" xmlns:ns3="a04c2f80-1bef-4486-925b-388b55f507c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="345f1e5c61c05e894262e6e3c1121887" ns2:_="" ns3:_="">
     <xsd:import namespace="3f799c52-a1b3-4ee5-ac1d-d25d561b6180"/>
@@ -6367,16 +6395,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC29259C-EA08-4B4D-9C83-622DD2E0263E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60CAEEA2-134A-46F0-9016-37BD8B8D32D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6393,7 +6420,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786CE926-E86C-4A2A-9112-C347C3BCF8D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6410,12 +6437,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC29259C-EA08-4B4D-9C83-622DD2E0263E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>